<commit_message>
add analysis of processing time
</commit_message>
<xml_diff>
--- a/otmm_decimal/time_compare_macpro.xlsx
+++ b/otmm_decimal/time_compare_macpro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\確率モデル\glycan\otmm_decimal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5454BE-DC27-4D9B-8330-6E8C4983289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BE6F23-C023-4898-AF86-17D260679F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440" xr2:uid="{6B34A1AE-571F-4A02-8490-45257AAE273A}"/>
   </bookViews>
@@ -84,12 +84,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -98,8 +113,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -117,6 +135,1164 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>エポック当たりの処理時間</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>単糖のみ</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.70731739463427856</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5539853053633057</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3770356358727192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.416853513102943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.415131699671406</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33.468408237883892</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.555309551581502</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.278640862918692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>188.70347163713913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EA36-4124-892F-A12D7816E08C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>単糖+結合様式</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.78068972455168284</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3736999544837314</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3427810030989118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.917197482336434</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.481096161861998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.882000965469665</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.005014125257624</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>133.52988394398571</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>290.8366934828</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EA36-4124-892F-A12D7816E08C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="22432576"/>
+        <c:axId val="22430080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="22432576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>データ数（個）</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22430080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="22430080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>処理時間（秒）</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22432576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75946957-FCB7-30E1-6225-9BD6AC7FAC95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011F8CE8-73A5-4783-B1AF-F45C7B9BE22A}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -428,269 +1604,293 @@
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>9.1951261302456206</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>13</v>
       </c>
-      <c r="D2">
-        <f>B2/C2</f>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D10" si="0">B2/C2</f>
         <v>0.70731739463427856</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>8.5875869700685108</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>11</v>
       </c>
-      <c r="I2">
-        <f>G2/H2</f>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I10" si="1">G2/H2</f>
         <v>0.78068972455168284</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>50</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>127.943470993079</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>36</v>
       </c>
-      <c r="D3">
-        <f>B3/C3</f>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
         <v>3.5539853053633057</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>50</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>179.321698133833</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>41</v>
       </c>
-      <c r="I3">
-        <f>G3/H3</f>
+      <c r="I3" s="1">
+        <f t="shared" si="1"/>
         <v>4.3736999544837314</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>100</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>236.06514034792701</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>32</v>
       </c>
-      <c r="D4">
-        <f>B4/C4</f>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
         <v>7.3770356358727192</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>317.65455410536299</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>34</v>
       </c>
-      <c r="I4">
-        <f>G4/H4</f>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
         <v>9.3427810030989118</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>200</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>295.50336323585299</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>18</v>
       </c>
-      <c r="D5">
-        <f>B5/C5</f>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
         <v>16.416853513102943</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>200</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>504.095542093738</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>23</v>
       </c>
-      <c r="I5">
-        <f>G5/H5</f>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
         <v>21.917197482336434</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>300</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>940.35987288784202</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>37</v>
       </c>
-      <c r="D6">
-        <f>B6/C6</f>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
         <v>25.415131699671406</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>300</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>482.73534626606801</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>14</v>
       </c>
-      <c r="I6">
-        <f>G6/H6</f>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
         <v>34.481096161861998</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>400</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>1204.86269656382</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>36</v>
       </c>
-      <c r="D7">
-        <f>B7/C7</f>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>33.468408237883892</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>400</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>1376.46002896409</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>30</v>
       </c>
-      <c r="I7">
-        <f>G7/H7</f>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
         <v>45.882000965469665</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>500</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>1702.2123820632601</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>40</v>
       </c>
-      <c r="D8">
-        <f>B8/C8</f>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
         <v>42.555309551581502</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>500</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>1281.1052966304101</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>21</v>
       </c>
-      <c r="I8">
-        <f>G8/H8</f>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
         <v>61.005014125257624</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>1000</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>2030.4087398471299</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>23</v>
       </c>
-      <c r="D9">
-        <f>B9/C9</f>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
         <v>88.278640862918692</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>1000</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>2804.1275628236999</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>21</v>
       </c>
-      <c r="I9">
-        <f>G9/H9</f>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
         <v>133.52988394398571</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>2000</v>
       </c>
-      <c r="F10">
+      <c r="B10" s="1">
+        <v>6415.9180356627303</v>
+      </c>
+      <c r="C10" s="1">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>188.70347163713913</v>
+      </c>
+      <c r="F10" s="1">
         <v>2000</v>
+      </c>
+      <c r="G10" s="1">
+        <v>10760.957658863599</v>
+      </c>
+      <c r="H10" s="1">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>290.8366934828</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change state_'set' into 'list', but there's no effect on the results
</commit_message>
<xml_diff>
--- a/otmm_decimal/time_compare_macpro.xlsx
+++ b/otmm_decimal/time_compare_macpro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\確率モデル\glycan\otmm_decimal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BE6F23-C023-4898-AF86-17D260679F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D699C375-11FE-4C1E-BE74-F96F9AE3F7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440" xr2:uid="{6B34A1AE-571F-4A02-8490-45257AAE273A}"/>
   </bookViews>
@@ -172,11 +172,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="ja-JP"/>
-              <a:t>1</a:t>
+              <a:t>OTMM</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>エポック当たりの処理時間</a:t>
+              <a:t>における１エポック当たりの処理時間</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1259,15 +1259,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1595,7 +1595,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
finish all of the tasks about my thesis:)
</commit_message>
<xml_diff>
--- a/otmm_decimal/time_compare_macpro.xlsx
+++ b/otmm_decimal/time_compare_macpro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\確率モデル\glycan\otmm_decimal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427885BE-D6B9-441E-BC06-B76827E7FEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6F4FEE-E635-43FC-B7C7-EEBA3B5F375C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440" xr2:uid="{6B34A1AE-571F-4A02-8490-45257AAE273A}"/>
   </bookViews>
@@ -1172,7 +1172,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2679,7 +2679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2690,7 +2690,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>